<commit_message>
spreadsheet needs second update
</commit_message>
<xml_diff>
--- a/missing_letters/Missing Letters Difficulty Levels.xlsx
+++ b/missing_letters/Missing Letters Difficulty Levels.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -62,46 +62,34 @@
     <t>Answer Representation</t>
   </si>
   <si>
-    <t>write.1.2.init.v.f.json</t>
+    <t>write.1.2.fin.v.f.json</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>vowel</t>
+  </si>
+  <si>
+    <t>common</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>write.1.2.fin.v.r.json</t>
+  </si>
+  <si>
+    <t>rare</t>
+  </si>
+  <si>
+    <t>write.1.3.init.c.f.json</t>
   </si>
   <si>
     <t>initial</t>
-  </si>
-  <si>
-    <t>vowel</t>
-  </si>
-  <si>
-    <t>common</t>
-  </si>
-  <si>
-    <t>Word</t>
-  </si>
-  <si>
-    <t>Write</t>
-  </si>
-  <si>
-    <t>write.1.2.init.v.r.json</t>
-  </si>
-  <si>
-    <t>rare</t>
-  </si>
-  <si>
-    <t>write.1.2.fin.v.f.json</t>
-  </si>
-  <si>
-    <t>final</t>
-  </si>
-  <si>
-    <t>write.1.2.fin.v.r.json</t>
-  </si>
-  <si>
-    <t>write.1.3.init.v.fjson</t>
-  </si>
-  <si>
-    <t>write.1.3.init.v.r.json</t>
-  </si>
-  <si>
-    <t>write.1.3.init.c.f.json</t>
   </si>
   <si>
     <t>consonant</t>
@@ -354,12 +342,12 @@
     <font>
       <b/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
     <font/>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -393,34 +381,34 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -510,10 +498,10 @@
         <v>14</v>
       </c>
       <c r="J2" s="7"/>
-      <c r="K2" s="4"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="4">
@@ -550,25 +538,25 @@
       <c r="B4" s="4">
         <v>3.0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1.0</v>
       </c>
-      <c r="D4" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="7"/>
@@ -576,38 +564,38 @@
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4">
         <v>4.0</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1.0</v>
       </c>
-      <c r="D5" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
+      <c r="A6" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="B6" s="4">
         <v>5.0</v>
@@ -637,8 +625,8 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
+      <c r="A7" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B7" s="4">
         <v>6.0</v>
@@ -668,8 +656,8 @@
       <c r="K7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
+      <c r="A8" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B8" s="4">
         <v>7.0</v>
@@ -681,10 +669,10 @@
         <v>3.0</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>12</v>
@@ -699,8 +687,8 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>24</v>
+      <c r="A9" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="4">
         <v>8.0</v>
@@ -712,10 +700,10 @@
         <v>3.0</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>16</v>
@@ -730,8 +718,8 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>25</v>
+      <c r="A10" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B10" s="4">
         <v>9.0</v>
@@ -743,7 +731,7 @@
         <v>3.0</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>11</v>
@@ -761,8 +749,8 @@
       <c r="K10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>26</v>
+      <c r="A11" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="B11" s="4">
         <v>10.0</v>
@@ -774,7 +762,7 @@
         <v>3.0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>11</v>
@@ -792,8 +780,8 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>27</v>
+      <c r="A12" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="4">
         <v>11.0</v>
@@ -802,13 +790,13 @@
         <v>1.0</v>
       </c>
       <c r="D12" s="4">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>12</v>
@@ -823,7 +811,7 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="4">
@@ -833,13 +821,13 @@
         <v>1.0</v>
       </c>
       <c r="D13" s="4">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>16</v>
@@ -854,7 +842,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="4">
@@ -864,10 +852,10 @@
         <v>1.0</v>
       </c>
       <c r="D14" s="4">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>11</v>
@@ -885,7 +873,7 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="4">
@@ -895,10 +883,10 @@
         <v>1.0</v>
       </c>
       <c r="D15" s="4">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>11</v>
@@ -916,7 +904,7 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="4">
@@ -932,7 +920,7 @@
         <v>10</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>12</v>
@@ -947,7 +935,7 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="4">
@@ -963,7 +951,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>16</v>
@@ -978,7 +966,7 @@
       <c r="K17" s="7"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="4">
@@ -991,7 +979,7 @@
         <v>4.0</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>11</v>
@@ -1009,7 +997,7 @@
       <c r="K18" s="7"/>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="9" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="4">
@@ -1022,7 +1010,7 @@
         <v>4.0</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>11</v>
@@ -1040,7 +1028,7 @@
       <c r="K19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="4">
@@ -1053,10 +1041,10 @@
         <v>4.0</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>12</v>
@@ -1071,7 +1059,7 @@
       <c r="K20" s="7"/>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="4">
@@ -1084,10 +1072,10 @@
         <v>4.0</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>16</v>
@@ -1102,7 +1090,7 @@
       <c r="K21" s="7"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="4">
@@ -1112,10 +1100,10 @@
         <v>1.0</v>
       </c>
       <c r="D22" s="4">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>11</v>
@@ -1133,7 +1121,7 @@
       <c r="K22" s="7"/>
     </row>
     <row r="23">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="4">
@@ -1143,10 +1131,10 @@
         <v>1.0</v>
       </c>
       <c r="D23" s="4">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>11</v>
@@ -1164,7 +1152,7 @@
       <c r="K23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="4">
@@ -1174,13 +1162,13 @@
         <v>1.0</v>
       </c>
       <c r="D24" s="4">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>12</v>
@@ -1195,7 +1183,7 @@
       <c r="K24" s="7"/>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="4">
@@ -1205,13 +1193,13 @@
         <v>1.0</v>
       </c>
       <c r="D25" s="4">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>16</v>
@@ -1226,7 +1214,7 @@
       <c r="K25" s="7"/>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="4">
@@ -1257,7 +1245,7 @@
       <c r="K26" s="7"/>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="4">
@@ -1288,7 +1276,7 @@
       <c r="K27" s="7"/>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="4">
@@ -1301,10 +1289,10 @@
         <v>5.0</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>12</v>
@@ -1332,10 +1320,10 @@
         <v>5.0</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>16</v>
@@ -1363,10 +1351,10 @@
         <v>5.0</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>12</v>
@@ -1394,10 +1382,10 @@
         <v>5.0</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>16</v>
@@ -1412,23 +1400,23 @@
       <c r="K31" s="7"/>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B32" s="4">
         <v>31.0</v>
       </c>
       <c r="C32" s="4">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D32" s="4">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>12</v>
@@ -1444,22 +1432,22 @@
     </row>
     <row r="33">
       <c r="A33" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B33" s="4">
         <v>32.0</v>
       </c>
       <c r="C33" s="4">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D33" s="4">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>16</v>
@@ -1475,22 +1463,22 @@
     </row>
     <row r="34">
       <c r="A34" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="4">
         <v>33.0</v>
       </c>
       <c r="C34" s="4">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D34" s="4">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>12</v>
@@ -1506,22 +1494,22 @@
     </row>
     <row r="35">
       <c r="A35" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B35" s="4">
         <v>34.0</v>
       </c>
       <c r="C35" s="4">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="D35" s="4">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>16</v>
@@ -1536,8 +1524,8 @@
       <c r="K35" s="7"/>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>52</v>
+      <c r="A36" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B36" s="4">
         <v>35.0</v>
@@ -1552,7 +1540,7 @@
         <v>10</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>12</v>
@@ -1567,8 +1555,8 @@
       <c r="K36" s="7"/>
     </row>
     <row r="37">
-      <c r="A37" s="3" t="s">
-        <v>54</v>
+      <c r="A37" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B37" s="4">
         <v>36.0</v>
@@ -1583,7 +1571,7 @@
         <v>10</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>16</v>
@@ -1598,8 +1586,8 @@
       <c r="K37" s="7"/>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="s">
-        <v>55</v>
+      <c r="A38" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="B38" s="4">
         <v>37.0</v>
@@ -1614,7 +1602,7 @@
         <v>10</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>12</v>
@@ -1629,7 +1617,7 @@
       <c r="K38" s="7"/>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="8" t="s">
         <v>57</v>
       </c>
       <c r="B39" s="4">
@@ -1645,7 +1633,7 @@
         <v>10</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>16</v>
@@ -1660,7 +1648,7 @@
       <c r="K39" s="7"/>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B40" s="4">
@@ -1673,10 +1661,10 @@
         <v>4.0</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>12</v>
@@ -1691,7 +1679,7 @@
       <c r="K40" s="7"/>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="8" t="s">
         <v>59</v>
       </c>
       <c r="B41" s="4">
@@ -1704,10 +1692,10 @@
         <v>4.0</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G41" s="4" t="s">
         <v>16</v>
@@ -1722,7 +1710,7 @@
       <c r="K41" s="7"/>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B42" s="4">
@@ -1735,10 +1723,10 @@
         <v>4.0</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G42" s="4" t="s">
         <v>12</v>
@@ -1753,7 +1741,7 @@
       <c r="K42" s="7"/>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B43" s="4">
@@ -1766,10 +1754,10 @@
         <v>4.0</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>16</v>
@@ -1784,7 +1772,7 @@
       <c r="K43" s="7"/>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="8" t="s">
         <v>62</v>
       </c>
       <c r="B44" s="4">
@@ -1794,13 +1782,13 @@
         <v>2.0</v>
       </c>
       <c r="D44" s="4">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>12</v>
@@ -1815,7 +1803,7 @@
       <c r="K44" s="7"/>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B45" s="4">
@@ -1825,13 +1813,13 @@
         <v>2.0</v>
       </c>
       <c r="D45" s="4">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>16</v>
@@ -1846,7 +1834,7 @@
       <c r="K45" s="7"/>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B46" s="4">
@@ -1856,13 +1844,13 @@
         <v>2.0</v>
       </c>
       <c r="D46" s="4">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>12</v>
@@ -1877,7 +1865,7 @@
       <c r="K46" s="7"/>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="8" t="s">
         <v>65</v>
       </c>
       <c r="B47" s="4">
@@ -1887,13 +1875,13 @@
         <v>2.0</v>
       </c>
       <c r="D47" s="4">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>16</v>
@@ -1908,7 +1896,7 @@
       <c r="K47" s="7"/>
     </row>
     <row r="48">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B48" s="4">
@@ -1924,7 +1912,7 @@
         <v>10</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>12</v>
@@ -1939,7 +1927,7 @@
       <c r="K48" s="7"/>
     </row>
     <row r="49">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B49" s="4">
@@ -1955,7 +1943,7 @@
         <v>10</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G49" s="4" t="s">
         <v>16</v>
@@ -1970,7 +1958,7 @@
       <c r="K49" s="7"/>
     </row>
     <row r="50">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="8" t="s">
         <v>68</v>
       </c>
       <c r="B50" s="4">
@@ -1986,7 +1974,7 @@
         <v>10</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G50" s="4" t="s">
         <v>12</v>
@@ -2001,7 +1989,7 @@
       <c r="K50" s="7"/>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B51" s="4">
@@ -2017,7 +2005,7 @@
         <v>10</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>16</v>
@@ -2032,7 +2020,7 @@
       <c r="K51" s="7"/>
     </row>
     <row r="52">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="8" t="s">
         <v>70</v>
       </c>
       <c r="B52" s="4">
@@ -2045,10 +2033,10 @@
         <v>5.0</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>12</v>
@@ -2063,7 +2051,7 @@
       <c r="K52" s="7"/>
     </row>
     <row r="53">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B53" s="4">
@@ -2076,10 +2064,10 @@
         <v>5.0</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G53" s="4" t="s">
         <v>16</v>
@@ -2094,7 +2082,7 @@
       <c r="K53" s="7"/>
     </row>
     <row r="54">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B54" s="4">
@@ -2107,10 +2095,10 @@
         <v>5.0</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G54" s="4" t="s">
         <v>12</v>
@@ -2125,7 +2113,7 @@
       <c r="K54" s="7"/>
     </row>
     <row r="55">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B55" s="4">
@@ -2138,10 +2126,10 @@
         <v>5.0</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G55" s="4" t="s">
         <v>16</v>
@@ -2156,23 +2144,23 @@
       <c r="K55" s="7"/>
     </row>
     <row r="56">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="8" t="s">
         <v>74</v>
       </c>
       <c r="B56" s="4">
         <v>55.0</v>
       </c>
       <c r="C56" s="4">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D56" s="4">
         <v>5.0</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>12</v>
@@ -2187,23 +2175,23 @@
       <c r="K56" s="7"/>
     </row>
     <row r="57">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="8" t="s">
         <v>75</v>
       </c>
       <c r="B57" s="4">
         <v>56.0</v>
       </c>
       <c r="C57" s="4">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D57" s="4">
         <v>5.0</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>16</v>
@@ -2218,23 +2206,23 @@
       <c r="K57" s="7"/>
     </row>
     <row r="58">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B58" s="4">
         <v>57.0</v>
       </c>
       <c r="C58" s="4">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D58" s="4">
         <v>5.0</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>12</v>
@@ -2249,23 +2237,23 @@
       <c r="K58" s="7"/>
     </row>
     <row r="59">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B59" s="4">
         <v>58.0</v>
       </c>
       <c r="C59" s="4">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D59" s="4">
         <v>5.0</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="G59" s="4" t="s">
         <v>16</v>
@@ -2280,7 +2268,7 @@
       <c r="K59" s="7"/>
     </row>
     <row r="60">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="8" t="s">
         <v>78</v>
       </c>
       <c r="B60" s="4">
@@ -2295,8 +2283,8 @@
       <c r="E60" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>56</v>
+      <c r="F60" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="G60" s="4" t="s">
         <v>12</v>
@@ -2311,7 +2299,7 @@
       <c r="K60" s="7"/>
     </row>
     <row r="61">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="8" t="s">
         <v>79</v>
       </c>
       <c r="B61" s="4">
@@ -2327,7 +2315,7 @@
         <v>10</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>16</v>
@@ -2342,7 +2330,7 @@
       <c r="K61" s="7"/>
     </row>
     <row r="62">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="8" t="s">
         <v>80</v>
       </c>
       <c r="B62" s="4">
@@ -2358,7 +2346,7 @@
         <v>10</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>12</v>
@@ -2373,7 +2361,7 @@
       <c r="K62" s="7"/>
     </row>
     <row r="63">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B63" s="4">
@@ -2389,7 +2377,7 @@
         <v>10</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>16</v>
@@ -2404,7 +2392,7 @@
       <c r="K63" s="7"/>
     </row>
     <row r="64">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="8" t="s">
         <v>82</v>
       </c>
       <c r="B64" s="4">
@@ -2417,10 +2405,10 @@
         <v>5.0</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>12</v>
@@ -2435,7 +2423,7 @@
       <c r="K64" s="7"/>
     </row>
     <row r="65">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="8" t="s">
         <v>83</v>
       </c>
       <c r="B65" s="4">
@@ -2448,10 +2436,10 @@
         <v>5.0</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>16</v>
@@ -2466,7 +2454,7 @@
       <c r="K65" s="7"/>
     </row>
     <row r="66">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="8" t="s">
         <v>84</v>
       </c>
       <c r="B66" s="4">
@@ -2479,10 +2467,10 @@
         <v>5.0</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>12</v>
@@ -2497,7 +2485,7 @@
       <c r="K66" s="7"/>
     </row>
     <row r="67">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="8" t="s">
         <v>85</v>
       </c>
       <c r="B67" s="4">
@@ -2510,10 +2498,10 @@
         <v>5.0</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>16</v>
@@ -2528,7 +2516,7 @@
       <c r="K67" s="7"/>
     </row>
     <row r="68">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="8" t="s">
         <v>86</v>
       </c>
       <c r="B68" s="4">
@@ -2538,13 +2526,13 @@
         <v>3.0</v>
       </c>
       <c r="D68" s="4">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F68" s="10" t="s">
-        <v>56</v>
+        <v>18</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>12</v>
@@ -2559,7 +2547,7 @@
       <c r="K68" s="7"/>
     </row>
     <row r="69">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="8" t="s">
         <v>87</v>
       </c>
       <c r="B69" s="4">
@@ -2569,13 +2557,13 @@
         <v>3.0</v>
       </c>
       <c r="D69" s="4">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>16</v>
@@ -2590,7 +2578,7 @@
       <c r="K69" s="7"/>
     </row>
     <row r="70">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="8" t="s">
         <v>88</v>
       </c>
       <c r="B70" s="4">
@@ -2600,13 +2588,13 @@
         <v>3.0</v>
       </c>
       <c r="D70" s="4">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>12</v>
@@ -2621,7 +2609,7 @@
       <c r="K70" s="7"/>
     </row>
     <row r="71">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="8" t="s">
         <v>89</v>
       </c>
       <c r="B71" s="4">
@@ -2631,13 +2619,13 @@
         <v>3.0</v>
       </c>
       <c r="D71" s="4">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>16</v>
@@ -2652,7 +2640,7 @@
       <c r="K71" s="7"/>
     </row>
     <row r="72">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="8" t="s">
         <v>90</v>
       </c>
       <c r="B72" s="4">
@@ -2667,8 +2655,8 @@
       <c r="E72" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F72" s="4" t="s">
-        <v>56</v>
+      <c r="F72" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>12</v>
@@ -2683,7 +2671,7 @@
       <c r="K72" s="7"/>
     </row>
     <row r="73">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="8" t="s">
         <v>91</v>
       </c>
       <c r="B73" s="4">
@@ -2699,7 +2687,7 @@
         <v>10</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>16</v>
@@ -2714,7 +2702,7 @@
       <c r="K73" s="7"/>
     </row>
     <row r="74">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="8" t="s">
         <v>92</v>
       </c>
       <c r="B74" s="4">
@@ -2730,7 +2718,7 @@
         <v>10</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>12</v>
@@ -2745,7 +2733,7 @@
       <c r="K74" s="7"/>
     </row>
     <row r="75">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="8" t="s">
         <v>93</v>
       </c>
       <c r="B75" s="4">
@@ -2761,7 +2749,7 @@
         <v>10</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>16</v>
@@ -2776,7 +2764,7 @@
       <c r="K75" s="7"/>
     </row>
     <row r="76">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="8" t="s">
         <v>94</v>
       </c>
       <c r="B76" s="4">
@@ -2789,10 +2777,10 @@
         <v>6.0</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>12</v>
@@ -2807,7 +2795,7 @@
       <c r="K76" s="7"/>
     </row>
     <row r="77">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="8" t="s">
         <v>95</v>
       </c>
       <c r="B77" s="4">
@@ -2820,10 +2808,10 @@
         <v>6.0</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>16</v>
@@ -2838,7 +2826,7 @@
       <c r="K77" s="7"/>
     </row>
     <row r="78">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="8" t="s">
         <v>96</v>
       </c>
       <c r="B78" s="4">
@@ -2851,10 +2839,10 @@
         <v>6.0</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>12</v>
@@ -2869,7 +2857,7 @@
       <c r="K78" s="7"/>
     </row>
     <row r="79">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="8" t="s">
         <v>97</v>
       </c>
       <c r="B79" s="4">
@@ -2882,10 +2870,10 @@
         <v>6.0</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>16</v>
@@ -2900,132 +2888,20 @@
       <c r="K79" s="7"/>
     </row>
     <row r="80">
-      <c r="A80" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B80" s="4">
-        <v>79.0</v>
-      </c>
-      <c r="C80" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="D80" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F80" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J80" s="7"/>
-      <c r="K80" s="7"/>
+      <c r="A80" s="11"/>
+      <c r="B80" s="12"/>
     </row>
     <row r="81">
-      <c r="A81" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B81" s="4">
-        <v>80.0</v>
-      </c>
-      <c r="C81" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="D81" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F81" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H81" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J81" s="7"/>
-      <c r="K81" s="7"/>
+      <c r="A81" s="11"/>
     </row>
     <row r="82">
-      <c r="A82" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B82" s="4">
-        <v>81.0</v>
-      </c>
-      <c r="C82" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="D82" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F82" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H82" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I82" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J82" s="7"/>
-      <c r="K82" s="7"/>
+      <c r="A82" s="11"/>
     </row>
     <row r="83">
-      <c r="A83" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B83" s="4">
-        <v>82.0</v>
-      </c>
-      <c r="C83" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="D83" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G83" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H83" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I83" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J83" s="7"/>
-      <c r="K83" s="7"/>
+      <c r="A83" s="11"/>
     </row>
     <row r="84">
       <c r="A84" s="11"/>
-      <c r="B84" s="12"/>
     </row>
     <row r="85">
       <c r="A85" s="11"/>
@@ -5834,18 +5710,6 @@
     </row>
     <row r="1020">
       <c r="A1020" s="11"/>
-    </row>
-    <row r="1021">
-      <c r="A1021" s="11"/>
-    </row>
-    <row r="1022">
-      <c r="A1022" s="11"/>
-    </row>
-    <row r="1023">
-      <c r="A1023" s="11"/>
-    </row>
-    <row r="1024">
-      <c r="A1024" s="11"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>

</xml_diff>